<commit_message>
Imagenes Bolsa y sellado
</commit_message>
<xml_diff>
--- a/Resultados Experimentales/Headspace/Resumen Headspace.xlsx
+++ b/Resultados Experimentales/Headspace/Resumen Headspace.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes-my.sharepoint.com/personal/df_rozo11_uniandes_edu_co/Documents/Duodecimo semestre/Repositorio_Maestria/Resultados Experimentales/Headspace/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="223" documentId="8_{22F2181A-421C-449B-9B87-A1B05CE41FE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{552781A9-AC02-4236-99DB-C75D523E6359}"/>
+  <xr:revisionPtr revIDLastSave="390" documentId="8_{22F2181A-421C-449B-9B87-A1B05CE41FE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1B4EA768-F535-4252-9398-E3EE17023088}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prueba 1 - Con Succión" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Miscelaneo " sheetId="5" r:id="rId5"/>
     <sheet name="Hoja1" sheetId="6" r:id="rId6"/>
     <sheet name="Hoja2" sheetId="7" r:id="rId7"/>
+    <sheet name="Headspace Bolsa" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="116">
   <si>
     <t>Destructivas</t>
   </si>
@@ -382,6 +383,33 @@
   </si>
   <si>
     <t>Sellado Maquina</t>
+  </si>
+  <si>
+    <t>Aceite Sin Luz- Frio</t>
+  </si>
+  <si>
+    <t>Aceite Sin Luz-Horno</t>
+  </si>
+  <si>
+    <t>Aceite Con Luz- Frio</t>
+  </si>
+  <si>
+    <t>Aceite Con Luz-Horno</t>
+  </si>
+  <si>
+    <t>Capsulas Sin Luz- Frio</t>
+  </si>
+  <si>
+    <t>Capsulas Con Luz- Frio</t>
+  </si>
+  <si>
+    <t>Capsulas Con Luz-Horno</t>
+  </si>
+  <si>
+    <t>Capsulas Sin Luz-Horno</t>
+  </si>
+  <si>
+    <t>Fecha - Hora</t>
   </si>
 </sst>
 </file>
@@ -830,7 +858,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1064,6 +1092,12 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1123,6 +1157,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -14987,20 +15024,20 @@
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B2" s="3"/>
-      <c r="C2" s="84" t="s">
+      <c r="C2" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="86"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B3" s="3" t="s">
@@ -15423,20 +15460,20 @@
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B13" s="1"/>
-      <c r="C13" s="84" t="s">
+      <c r="C13" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="84"/>
-      <c r="E13" s="84"/>
-      <c r="F13" s="84"/>
-      <c r="G13" s="84"/>
-      <c r="H13" s="84"/>
-      <c r="I13" s="84"/>
-      <c r="J13" s="84"/>
-      <c r="K13" s="84"/>
-      <c r="L13" s="84"/>
-      <c r="M13" s="84"/>
-      <c r="N13" s="84"/>
+      <c r="D13" s="86"/>
+      <c r="E13" s="86"/>
+      <c r="F13" s="86"/>
+      <c r="G13" s="86"/>
+      <c r="H13" s="86"/>
+      <c r="I13" s="86"/>
+      <c r="J13" s="86"/>
+      <c r="K13" s="86"/>
+      <c r="L13" s="86"/>
+      <c r="M13" s="86"/>
+      <c r="N13" s="86"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B14" s="3" t="s">
@@ -15848,10 +15885,10 @@
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B24" s="83" t="s">
+      <c r="B24" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="83"/>
+      <c r="C24" s="85"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B25" s="3" t="s">
@@ -15925,79 +15962,79 @@
   <sheetData>
     <row r="1" spans="1:33" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="1:33" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="D2" s="87" t="s">
+      <c r="D2" s="89" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="88"/>
-      <c r="N2" s="88"/>
-      <c r="O2" s="88"/>
-      <c r="P2" s="88"/>
-      <c r="Q2" s="88"/>
-      <c r="R2" s="88"/>
-      <c r="S2" s="88"/>
-      <c r="T2" s="88"/>
-      <c r="U2" s="89"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
+      <c r="O2" s="90"/>
+      <c r="P2" s="90"/>
+      <c r="Q2" s="90"/>
+      <c r="R2" s="90"/>
+      <c r="S2" s="90"/>
+      <c r="T2" s="90"/>
+      <c r="U2" s="91"/>
     </row>
     <row r="3" spans="1:33" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="85"/>
-      <c r="C3" s="86"/>
-      <c r="D3" s="93" t="s">
+      <c r="B3" s="87"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="95" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="94"/>
-      <c r="F3" s="94"/>
-      <c r="G3" s="94" t="s">
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="94"/>
-      <c r="I3" s="94"/>
-      <c r="J3" s="94" t="s">
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="96" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="94"/>
-      <c r="L3" s="94"/>
-      <c r="M3" s="95" t="s">
+      <c r="K3" s="96"/>
+      <c r="L3" s="96"/>
+      <c r="M3" s="97" t="s">
         <v>32</v>
       </c>
-      <c r="N3" s="95"/>
-      <c r="O3" s="95"/>
-      <c r="P3" s="95" t="s">
+      <c r="N3" s="97"/>
+      <c r="O3" s="97"/>
+      <c r="P3" s="97" t="s">
         <v>33</v>
       </c>
-      <c r="Q3" s="95"/>
-      <c r="R3" s="95"/>
-      <c r="S3" s="94" t="s">
+      <c r="Q3" s="97"/>
+      <c r="R3" s="97"/>
+      <c r="S3" s="96" t="s">
         <v>34</v>
       </c>
-      <c r="T3" s="94"/>
-      <c r="U3" s="96"/>
-      <c r="V3" s="90" t="s">
+      <c r="T3" s="96"/>
+      <c r="U3" s="98"/>
+      <c r="V3" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="W3" s="91"/>
-      <c r="X3" s="91"/>
-      <c r="Y3" s="91"/>
-      <c r="Z3" s="91"/>
-      <c r="AA3" s="92"/>
-      <c r="AB3" s="90" t="s">
+      <c r="W3" s="93"/>
+      <c r="X3" s="93"/>
+      <c r="Y3" s="93"/>
+      <c r="Z3" s="93"/>
+      <c r="AA3" s="94"/>
+      <c r="AB3" s="92" t="s">
         <v>51</v>
       </c>
-      <c r="AC3" s="91"/>
-      <c r="AD3" s="91"/>
-      <c r="AE3" s="91"/>
-      <c r="AF3" s="91"/>
-      <c r="AG3" s="92"/>
+      <c r="AC3" s="93"/>
+      <c r="AD3" s="93"/>
+      <c r="AE3" s="93"/>
+      <c r="AF3" s="93"/>
+      <c r="AG3" s="94"/>
     </row>
     <row r="4" spans="1:33" s="20" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="23" t="s">
@@ -17171,24 +17208,24 @@
   <sheetData>
     <row r="2" spans="2:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="3" spans="2:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="F3" s="97" t="s">
+      <c r="F3" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98" t="s">
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100" t="s">
         <v>55</v>
       </c>
-      <c r="J3" s="98"/>
-      <c r="K3" s="99"/>
-      <c r="L3" s="97" t="s">
+      <c r="J3" s="100"/>
+      <c r="K3" s="101"/>
+      <c r="L3" s="99" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="99"/>
-      <c r="N3" s="97" t="s">
+      <c r="M3" s="101"/>
+      <c r="N3" s="99" t="s">
         <v>18</v>
       </c>
-      <c r="O3" s="99"/>
+      <c r="O3" s="101"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.45">
       <c r="B4" s="42"/>
@@ -17640,7 +17677,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C40DBE8-B731-453D-9237-4B31BC596AD3}">
   <dimension ref="B3:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+    <sheetView topLeftCell="C4" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -17667,24 +17704,24 @@
       <c r="C4" s="20"/>
       <c r="D4" s="20"/>
       <c r="E4" s="20"/>
-      <c r="F4" s="97" t="s">
+      <c r="F4" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="G4" s="98"/>
-      <c r="H4" s="99"/>
-      <c r="I4" s="97" t="s">
+      <c r="G4" s="100"/>
+      <c r="H4" s="101"/>
+      <c r="I4" s="99" t="s">
         <v>55</v>
       </c>
-      <c r="J4" s="98"/>
-      <c r="K4" s="99"/>
-      <c r="L4" s="97" t="s">
+      <c r="J4" s="100"/>
+      <c r="K4" s="101"/>
+      <c r="L4" s="99" t="s">
         <v>18</v>
       </c>
-      <c r="M4" s="99"/>
-      <c r="N4" s="97" t="s">
+      <c r="M4" s="101"/>
+      <c r="N4" s="99" t="s">
         <v>83</v>
       </c>
-      <c r="O4" s="99"/>
+      <c r="O4" s="101"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.45">
       <c r="B5" s="60"/>
@@ -18062,14 +18099,14 @@
   <sheetData>
     <row r="1" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="F2" s="100" t="s">
+      <c r="F2" s="102" t="s">
         <v>60</v>
       </c>
-      <c r="G2" s="101"/>
-      <c r="H2" s="101"/>
-      <c r="I2" s="101"/>
-      <c r="J2" s="101"/>
-      <c r="K2" s="102"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="103"/>
+      <c r="I2" s="103"/>
+      <c r="J2" s="103"/>
+      <c r="K2" s="104"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B3" s="51"/>
@@ -18889,91 +18926,442 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Is_Collaboration_Space_Locked xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
-    <Invited_Teachers xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
-    <IsNotebookLocked xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
-    <Teachers xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Teachers>
-    <Distribution_Groups xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
-    <Self_Registration_Enabled xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
-    <LMS_Mappings xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
-    <FolderType xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
-    <CultureName xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
-    <Templates xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
-    <Has_Teacher_Only_SectionGroup xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
-    <Members xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Members>
-    <Member_Groups xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Member_Groups>
-    <NotebookType xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
-    <Leaders xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Leaders>
-    <Has_Leaders_Only_SectionGroup xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
-    <Owner xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <Math_Settings xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
-    <DefaultSectionNames xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
-    <Invited_Members xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
-    <AppVersion xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
-    <TeamsChannelId xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
-    <Invited_Students xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
-    <Invited_Leaders xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
-    <Students xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Students>
-    <Student_Groups xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Student_Groups>
-  </documentManagement>
-</p:properties>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68FCB3BF-D5D7-4386-9A75-AB641F79C58D}">
+  <dimension ref="A2:AC6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AB7" sqref="AB7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="16.3984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="C2" s="105" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" s="105"/>
+      <c r="E2" s="105"/>
+      <c r="F2" s="105" t="s">
+        <v>108</v>
+      </c>
+      <c r="G2" s="105"/>
+      <c r="H2" s="105"/>
+      <c r="I2" s="105" t="s">
+        <v>109</v>
+      </c>
+      <c r="J2" s="105"/>
+      <c r="K2" s="105"/>
+      <c r="L2" s="105" t="s">
+        <v>110</v>
+      </c>
+      <c r="M2" s="105"/>
+      <c r="N2" s="105"/>
+      <c r="O2" s="105" t="s">
+        <v>111</v>
+      </c>
+      <c r="P2" s="105"/>
+      <c r="Q2" s="105"/>
+      <c r="R2" s="105" t="s">
+        <v>114</v>
+      </c>
+      <c r="S2" s="105"/>
+      <c r="T2" s="105"/>
+      <c r="U2" s="105" t="s">
+        <v>112</v>
+      </c>
+      <c r="V2" s="105"/>
+      <c r="W2" s="105"/>
+      <c r="X2" s="105" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y2" s="105"/>
+      <c r="Z2" s="105"/>
+      <c r="AA2" s="105" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB2" s="105"/>
+      <c r="AC2" s="105"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="A3" s="83" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" s="83" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>3</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>2</v>
+      </c>
+      <c r="N3">
+        <v>3</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>2</v>
+      </c>
+      <c r="Q3">
+        <v>3</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>2</v>
+      </c>
+      <c r="T3">
+        <v>3</v>
+      </c>
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3">
+        <v>2</v>
+      </c>
+      <c r="W3">
+        <v>3</v>
+      </c>
+      <c r="X3">
+        <v>1</v>
+      </c>
+      <c r="Y3">
+        <v>2</v>
+      </c>
+      <c r="Z3">
+        <v>3</v>
+      </c>
+      <c r="AA3">
+        <v>1</v>
+      </c>
+      <c r="AB3">
+        <v>2</v>
+      </c>
+      <c r="AC3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="A4" s="84">
+        <v>44134.71875</v>
+      </c>
+      <c r="B4" s="83">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>20.5</v>
+      </c>
+      <c r="D4">
+        <v>20.5</v>
+      </c>
+      <c r="E4">
+        <v>20.5</v>
+      </c>
+      <c r="F4">
+        <v>20.5</v>
+      </c>
+      <c r="G4">
+        <v>20.5</v>
+      </c>
+      <c r="H4">
+        <v>20.5</v>
+      </c>
+      <c r="I4">
+        <v>20.5</v>
+      </c>
+      <c r="J4">
+        <v>20.5</v>
+      </c>
+      <c r="K4">
+        <v>20.5</v>
+      </c>
+      <c r="L4">
+        <v>20.5</v>
+      </c>
+      <c r="M4">
+        <v>20.5</v>
+      </c>
+      <c r="N4">
+        <v>20.5</v>
+      </c>
+      <c r="O4">
+        <v>20.5</v>
+      </c>
+      <c r="P4">
+        <v>20.5</v>
+      </c>
+      <c r="Q4">
+        <v>20.5</v>
+      </c>
+      <c r="R4">
+        <v>20.5</v>
+      </c>
+      <c r="S4">
+        <v>20.5</v>
+      </c>
+      <c r="T4">
+        <v>20.5</v>
+      </c>
+      <c r="U4">
+        <v>20.5</v>
+      </c>
+      <c r="V4">
+        <v>20.5</v>
+      </c>
+      <c r="W4">
+        <v>20.5</v>
+      </c>
+      <c r="X4">
+        <v>20.5</v>
+      </c>
+      <c r="Y4">
+        <v>20.5</v>
+      </c>
+      <c r="Z4">
+        <v>20.5</v>
+      </c>
+      <c r="AA4">
+        <v>20.5</v>
+      </c>
+      <c r="AB4">
+        <v>20.5</v>
+      </c>
+      <c r="AC4">
+        <v>20.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="A5" s="84">
+        <v>44138.375</v>
+      </c>
+      <c r="B5" s="83">
+        <f>(A5-$A$4)*24</f>
+        <v>87.75</v>
+      </c>
+      <c r="C5">
+        <v>20.6</v>
+      </c>
+      <c r="D5">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="E5">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="F5">
+        <v>20.5</v>
+      </c>
+      <c r="G5">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="H5">
+        <v>20.6</v>
+      </c>
+      <c r="I5">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="J5">
+        <v>20.6</v>
+      </c>
+      <c r="K5">
+        <v>20.6</v>
+      </c>
+      <c r="L5">
+        <v>20.6</v>
+      </c>
+      <c r="M5">
+        <v>20.5</v>
+      </c>
+      <c r="N5">
+        <v>20.6</v>
+      </c>
+      <c r="O5">
+        <v>20.6</v>
+      </c>
+      <c r="P5">
+        <v>20.6</v>
+      </c>
+      <c r="Q5">
+        <v>20.6</v>
+      </c>
+      <c r="R5">
+        <v>20.6</v>
+      </c>
+      <c r="S5">
+        <v>20.6</v>
+      </c>
+      <c r="T5">
+        <v>20.6</v>
+      </c>
+      <c r="U5">
+        <v>20.6</v>
+      </c>
+      <c r="V5">
+        <v>20.6</v>
+      </c>
+      <c r="W5">
+        <v>20.6</v>
+      </c>
+      <c r="X5">
+        <v>20.6</v>
+      </c>
+      <c r="Y5">
+        <v>20.6</v>
+      </c>
+      <c r="Z5">
+        <v>20.6</v>
+      </c>
+      <c r="AA5">
+        <v>20.6</v>
+      </c>
+      <c r="AB5">
+        <v>20.6</v>
+      </c>
+      <c r="AC5">
+        <v>20.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="A6" s="84">
+        <v>44139.354166666664</v>
+      </c>
+      <c r="B6" s="83">
+        <f>(A6-$A$4)*24</f>
+        <v>111.24999999994179</v>
+      </c>
+      <c r="C6">
+        <v>20.6</v>
+      </c>
+      <c r="D6">
+        <v>20.6</v>
+      </c>
+      <c r="E6">
+        <v>20.6</v>
+      </c>
+      <c r="F6">
+        <v>20.6</v>
+      </c>
+      <c r="G6">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="H6">
+        <v>20.6</v>
+      </c>
+      <c r="I6">
+        <v>20.6</v>
+      </c>
+      <c r="J6">
+        <v>20.6</v>
+      </c>
+      <c r="K6">
+        <v>20.6</v>
+      </c>
+      <c r="L6">
+        <v>20.6</v>
+      </c>
+      <c r="M6">
+        <v>20.6</v>
+      </c>
+      <c r="N6">
+        <v>20.6</v>
+      </c>
+      <c r="O6">
+        <v>20.6</v>
+      </c>
+      <c r="P6">
+        <v>20.6</v>
+      </c>
+      <c r="Q6">
+        <v>20.6</v>
+      </c>
+      <c r="R6">
+        <v>20.6</v>
+      </c>
+      <c r="S6">
+        <v>20.6</v>
+      </c>
+      <c r="T6">
+        <v>20.6</v>
+      </c>
+      <c r="U6">
+        <v>20.6</v>
+      </c>
+      <c r="V6">
+        <v>20.6</v>
+      </c>
+      <c r="W6">
+        <v>20.6</v>
+      </c>
+      <c r="X6">
+        <v>20.6</v>
+      </c>
+      <c r="Y6">
+        <v>20.6</v>
+      </c>
+      <c r="Z6">
+        <v>20.6</v>
+      </c>
+      <c r="AA6">
+        <v>20.6</v>
+      </c>
+      <c r="AB6">
+        <v>20.6</v>
+      </c>
+      <c r="AC6">
+        <v>20.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="U2:W2"/>
+    <mergeCell ref="X2:Z2"/>
+    <mergeCell ref="AA2:AC2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="R2:T2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101006E073622718B7D418B69CBE92FF13C49" ma:contentTypeVersion="39" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="5f1dbbd8d2bc6d63873560f8f91a64fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2d185e16-06da-45ab-8500-654d664b7dd3" xmlns:ns4="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0256b4d38701b5e0b7a2941a706499e5" ns3:_="" ns4:_="">
     <xsd:import namespace="2d185e16-06da-45ab-8500-654d664b7dd3"/>
@@ -19466,25 +19854,91 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{09AB5318-E418-4B62-9E51-22DF6F108056}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A60FE89-AD0C-4ABB-8D67-D409A26F781F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Is_Collaboration_Space_Locked xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
+    <Invited_Teachers xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
+    <IsNotebookLocked xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
+    <Teachers xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Teachers>
+    <Distribution_Groups xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
+    <Self_Registration_Enabled xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
+    <LMS_Mappings xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
+    <FolderType xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
+    <CultureName xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
+    <Templates xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
+    <Has_Teacher_Only_SectionGroup xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
+    <Members xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Members>
+    <Member_Groups xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Member_Groups>
+    <NotebookType xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
+    <Leaders xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Leaders>
+    <Has_Leaders_Only_SectionGroup xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
+    <Owner xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <Math_Settings xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
+    <DefaultSectionNames xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
+    <Invited_Members xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
+    <AppVersion xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
+    <TeamsChannelId xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
+    <Invited_Students xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
+    <Invited_Leaders xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
+    <Students xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Students>
+    <Student_Groups xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Student_Groups>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8A38F03-A22E-4DB2-8B79-1B7E6B581CEF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -19501,4 +19955,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A60FE89-AD0C-4ABB-8D67-D409A26F781F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{09AB5318-E418-4B62-9E51-22DF6F108056}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>